<commit_message>
final changes in all codes: shipment merging, shipment graphing, overdose graphing, and summary statistics. adds new labels to graphs and uses the latest county data with missing values filled in
</commit_message>
<xml_diff>
--- a/20_intermediate_files/drug_shipment_summary_table.xlsx
+++ b/20_intermediate_files/drug_shipment_summary_table.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
+  <si>
+    <t>FIPS</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
   <si>
     <t>Total_Weight</t>
   </si>
@@ -404,13 +413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,116 +429,197 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>6010</v>
+        <v>3548</v>
       </c>
       <c r="C2">
-        <v>6010</v>
+        <v>3548</v>
       </c>
       <c r="D2">
-        <v>6010</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>3548</v>
+      </c>
+      <c r="E2">
+        <v>3548</v>
+      </c>
+      <c r="F2">
+        <v>3548</v>
+      </c>
+      <c r="G2">
+        <v>3548</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>36242.54343074636</v>
+        <v>1773.5</v>
       </c>
       <c r="C3">
-        <v>89461.33910149751</v>
+        <v>23018.95180383314</v>
       </c>
       <c r="D3">
-        <v>35156.58652911791</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>2009.000563697858</v>
+      </c>
+      <c r="E3">
+        <v>48278.40100452794</v>
+      </c>
+      <c r="F3">
+        <v>92301.42390078917</v>
+      </c>
+      <c r="G3">
+        <v>41952.45182851247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>126062.9674828069</v>
+        <v>1024.363704940779</v>
       </c>
       <c r="C4">
-        <v>257257.8151228494</v>
+        <v>16271.50384454539</v>
       </c>
       <c r="D4">
-        <v>27564.59781531489</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>2.00112731638899</v>
+      </c>
+      <c r="E4">
+        <v>156986.4201255817</v>
+      </c>
+      <c r="F4">
+        <v>204117.6904437121</v>
+      </c>
+      <c r="G4">
+        <v>31513.92345649195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1001</v>
+      </c>
+      <c r="D5">
+        <v>2006</v>
+      </c>
+      <c r="E5">
         <v>0.3027</v>
       </c>
-      <c r="C5">
+      <c r="F5">
         <v>2893</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>10.46318700311096</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>3131.641341749994</v>
+        <v>886.75</v>
       </c>
       <c r="C6">
-        <v>15093.75</v>
+        <v>12121</v>
       </c>
       <c r="D6">
-        <v>17310.20568447091</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>2007</v>
+      </c>
+      <c r="E6">
+        <v>4341.690424250019</v>
+      </c>
+      <c r="F6">
+        <v>16846</v>
+      </c>
+      <c r="G6">
+        <v>21230.24606345244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>9201.453870000118</v>
+        <v>1773.5</v>
       </c>
       <c r="C7">
-        <v>27558</v>
+        <v>13253</v>
       </c>
       <c r="D7">
-        <v>27890.02287269812</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>2009</v>
+      </c>
+      <c r="E7">
+        <v>11998.83888182528</v>
+      </c>
+      <c r="F7">
+        <v>29479.5</v>
+      </c>
+      <c r="G7">
+        <v>34115.93639706657</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>26733.4788799634</v>
+        <v>2660.25</v>
       </c>
       <c r="C8">
-        <v>67088.5</v>
+        <v>45027</v>
       </c>
       <c r="D8">
-        <v>45026.65660572747</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>2011</v>
+      </c>
+      <c r="E8">
+        <v>35026.13619929253</v>
+      </c>
+      <c r="F8">
+        <v>74864.75</v>
+      </c>
+      <c r="G8">
+        <v>52642.51799479323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9">
+        <v>3547</v>
+      </c>
+      <c r="C9">
+        <v>47189</v>
+      </c>
+      <c r="D9">
+        <v>2012</v>
+      </c>
+      <c r="E9">
         <v>3026736.844583195</v>
       </c>
-      <c r="C9">
-        <v>5239351</v>
-      </c>
-      <c r="D9">
+      <c r="F9">
+        <v>2576554</v>
+      </c>
+      <c r="G9">
         <v>263276.1895904924</v>
       </c>
     </row>

</xml_diff>